<commit_message>
Arreglado la edicion de citas
</commit_message>
<xml_diff>
--- a/MANUAL TECNICO/Backlog_7245.xlsx
+++ b/MANUAL TECNICO/Backlog_7245.xlsx
@@ -133,40 +133,40 @@
     <t>Inicio de sesión</t>
   </si>
   <si>
+    <t>Semana 4</t>
+  </si>
+  <si>
+    <t>HU-03</t>
+  </si>
+  <si>
+    <t>Edición de perfil de usuario</t>
+  </si>
+  <si>
+    <t>HU-04</t>
+  </si>
+  <si>
+    <t>Agendamiento de cita</t>
+  </si>
+  <si>
+    <t>Semana 5</t>
+  </si>
+  <si>
+    <t>16 horas</t>
+  </si>
+  <si>
+    <t>HU-05</t>
+  </si>
+  <si>
+    <t>Modificación de cita</t>
+  </si>
+  <si>
+    <t>HU-06</t>
+  </si>
+  <si>
+    <t>Recordatorios de citas</t>
+  </si>
+  <si>
     <t>Por hacer</t>
-  </si>
-  <si>
-    <t>Semana 4</t>
-  </si>
-  <si>
-    <t>HU-03</t>
-  </si>
-  <si>
-    <t>Edición de perfil de usuario</t>
-  </si>
-  <si>
-    <t>HU-04</t>
-  </si>
-  <si>
-    <t>Agendamiento de cita</t>
-  </si>
-  <si>
-    <t>Semana 5</t>
-  </si>
-  <si>
-    <t>16 horas</t>
-  </si>
-  <si>
-    <t>HU-05</t>
-  </si>
-  <si>
-    <t>Modificación de cita</t>
-  </si>
-  <si>
-    <t>HU-06</t>
-  </si>
-  <si>
-    <t>Recordatorios de citas</t>
   </si>
   <si>
     <t>Semana 6</t>
@@ -384,7 +384,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -958,10 +958,10 @@
         <v>30</v>
       </c>
       <c r="H9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>34</v>
@@ -972,10 +972,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>32</v>
@@ -990,7 +990,7 @@
         <v>30</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
@@ -1000,10 +1000,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>32</v>
@@ -1018,13 +1018,13 @@
         <v>30</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="I11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
@@ -1032,10 +1032,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>32</v>
@@ -1047,10 +1047,10 @@
         <v>15</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -1060,10 +1060,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>32</v>
@@ -1075,10 +1075,10 @@
         <v>15</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>51</v>
@@ -1107,10 +1107,10 @@
         <v>15</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -1138,7 +1138,7 @@
         <v>52</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>57</v>
@@ -1170,7 +1170,7 @@
         <v>52</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
@@ -1198,7 +1198,7 @@
         <v>58</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>

</xml_diff>

<commit_message>
Hasta qui final 2.0
</commit_message>
<xml_diff>
--- a/MANUAL TECNICO/Backlog_7245.xlsx
+++ b/MANUAL TECNICO/Backlog_7245.xlsx
@@ -175,7 +175,7 @@
     <t>HU-07</t>
   </si>
   <si>
-    <t>Registro de información clínica</t>
+    <t>Generación de carnet de vacunación</t>
   </si>
   <si>
     <t>8 horas</t>
@@ -184,7 +184,7 @@
     <t>HU-08</t>
   </si>
   <si>
-    <t>Generación de carnet de vacunación</t>
+    <t>Registro de información clínica-vacunas</t>
   </si>
   <si>
     <t>Semana 7</t>
@@ -995,7 +995,7 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -1055,7 +1055,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -1115,7 +1115,7 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -1175,7 +1175,7 @@
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="21">
       <c r="A17" s="6">
         <v>15</v>
       </c>

</xml_diff>